<commit_message>
Update to figures and new analysis
</commit_message>
<xml_diff>
--- a/docs/amps_prediction.xlsx
+++ b/docs/amps_prediction.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome_2025/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131315E1-764E-2D4F-9641-CAF20AF128CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A36E8EC-E99B-EE41-92AD-197570EEFC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{D0FE8B26-41E0-2A46-B2EA-AAB3A158C054}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{D0FE8B26-41E0-2A46-B2EA-AAB3A158C054}"/>
   </bookViews>
   <sheets>
     <sheet name="420_AMPs" sheetId="1" r:id="rId1"/>
     <sheet name="193_AMPs" sheetId="2" r:id="rId2"/>
     <sheet name="133_AMPs" sheetId="5" r:id="rId3"/>
     <sheet name="114_AMPs" sheetId="3" r:id="rId4"/>
-    <sheet name="9_AMPs" sheetId="4" r:id="rId5"/>
+    <sheet name="112_AMPs" sheetId="6" r:id="rId5"/>
+    <sheet name="9_AMPs" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="1625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4992" uniqueCount="1625">
   <si>
     <t>transcript_id</t>
   </si>
@@ -18252,8 +18253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D924C1-C05E-8D45-B73D-061AF6330212}">
   <dimension ref="A1:O342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22517,18 +22518,4283 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A837C33-E513-FD45-9224-A40C02E07EC8}">
+  <dimension ref="A1:O342"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1459</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1460</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1618</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1619</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C2" t="s">
+        <v>843</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1430</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>842</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1457</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1577</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>1395</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D4">
+        <v>53</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1425</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1580</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>1471</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1617</v>
+      </c>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>660</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1448</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>1407</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1620</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>734</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D6">
+        <v>66</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>1395</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>659</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1583</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>1401</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>658</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1562</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>1613</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>715</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D9">
+        <v>81</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>568</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D10">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>1481</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>1397</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>665</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>579</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D12">
+        <v>68</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>1395</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
+        <v>684</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1605</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
+        <v>691</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D14">
+        <v>44</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1563</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1487</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>461</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>594</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1567</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>1391</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" t="s">
+        <v>696</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D18">
+        <v>79</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s">
+        <v>697</v>
+      </c>
+      <c r="C19" t="s">
+        <v>882</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>550</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D20">
+        <v>35</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1596</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>551</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>781</v>
+      </c>
+      <c r="C22" t="s">
+        <v>887</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>1456</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>1495</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>1414</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" t="s">
+        <v>762</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D23">
+        <v>47</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1563</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>1497</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
+        <v>695</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D24">
+        <v>32</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1570</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" t="s">
+        <v>753</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D25">
+        <v>72</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1566</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>1501</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" t="s">
+        <v>737</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D26">
+        <v>66</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1563</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>1502</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>595</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>1503</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>1409</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>614</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D28">
+        <v>24</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1598</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>1505</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>615</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D29">
+        <v>33</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1608</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>1417</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>809</v>
+      </c>
+      <c r="C30" t="s">
+        <v>901</v>
+      </c>
+      <c r="D30">
+        <v>96</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" t="s">
+        <v>763</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D31">
+        <v>97</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1564</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>1502</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>526</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>1435</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1600</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>1510</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>1415</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>493</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D33">
+        <v>74</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1607</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" t="s">
+        <v>765</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D34">
+        <v>84</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" t="s">
+        <v>766</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D35">
+        <v>71</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>612</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D36">
+        <v>17</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>611</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D37">
+        <v>71</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1593</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" t="s">
+        <v>642</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D38">
+        <v>13</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>1443</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1606</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>1622</v>
+      </c>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
+        <v>742</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1602</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>1464</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>1615</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>1623</v>
+      </c>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s">
+        <v>655</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D40">
+        <v>76</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1588</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>1518</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>656</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D41">
+        <v>76</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1588</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>1518</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>745</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D42">
+        <v>27</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" t="s">
+        <v>750</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D43">
+        <v>22</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" t="s">
+        <v>757</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D44">
+        <v>42</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1610</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>1523</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>1418</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>599</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>429</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>1526</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>1387</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="O46" s="3"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>430</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D47">
+        <v>12</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1601</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>1528</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>1416</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>459</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D48">
+        <v>11</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1597</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>1505</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="O48" s="3"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>458</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D49">
+        <v>50</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>496</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D50">
+        <v>41</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="O50" s="3"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
+        <v>495</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D51">
+        <v>76</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1568</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s">
+        <v>727</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D52">
+        <v>37</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>1394</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" t="s">
+        <v>732</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D53">
+        <v>22</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1604</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" t="s">
+        <v>729</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D54">
+        <v>42</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1609</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>1417</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>434</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D55">
+        <v>13</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>436</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D56">
+        <v>13</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
+        <v>448</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D57">
+        <v>91</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>443</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D58">
+        <v>22</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1611</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" t="s">
+        <v>610</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D59">
+        <v>46</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1578</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>1396</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" t="s">
+        <v>739</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D60">
+        <v>34</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="s">
+        <v>553</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D61">
+        <v>20</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>1538</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>1616</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" t="s">
+        <v>726</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D62">
+        <v>24</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1607</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>651</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D63">
+        <v>20</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1567</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" t="s">
+        <v>571</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D64">
+        <v>50</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1572</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" t="s">
+        <v>570</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D65">
+        <v>29</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>1438</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1569</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" t="s">
+        <v>646</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D66">
+        <v>27</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" t="s">
+        <v>645</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D67">
+        <v>10</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D68" s="1">
+        <v>21</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H68" s="7" t="s">
+        <v>1613</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" t="s">
+        <v>708</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D69">
+        <v>15</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1595</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" t="s">
+        <v>710</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D70">
+        <v>14</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>1452</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" t="s">
+        <v>511</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D71">
+        <v>41</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" t="s">
+        <v>510</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D72">
+        <v>21</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>1420</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>43</v>
+      </c>
+      <c r="B73" t="s">
+        <v>514</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D73">
+        <v>13</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" t="s">
+        <v>515</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D74">
+        <v>17</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1570</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" t="s">
+        <v>508</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D75">
+        <v>39</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" t="s">
+        <v>505</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D76">
+        <v>20</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F76" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" t="s">
+        <v>668</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D77">
+        <v>26</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F77" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" t="s">
+        <v>671</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D78">
+        <v>10</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" t="s">
+        <v>669</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D79">
+        <v>70</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F79" t="s">
+        <v>1604</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>121</v>
+      </c>
+      <c r="B80" t="s">
+        <v>674</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D80">
+        <v>22</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" t="s">
+        <v>675</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D81">
+        <v>22</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>123</v>
+      </c>
+      <c r="B82" t="s">
+        <v>676</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D82">
+        <v>14</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>124</v>
+      </c>
+      <c r="B83" t="s">
+        <v>677</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D83">
+        <v>11</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" t="s">
+        <v>792</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D84">
+        <v>24</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>1546</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>1412</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>789</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D85">
+        <v>31</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86" t="s">
+        <v>488</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D86">
+        <v>29</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" t="s">
+        <v>585</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D87">
+        <v>40</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88" t="s">
+        <v>541</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D88">
+        <v>29</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>1420</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" t="s">
+        <v>542</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D89">
+        <v>29</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>1420</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>50</v>
+      </c>
+      <c r="B90" t="s">
+        <v>528</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D90">
+        <v>73</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1567</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>51</v>
+      </c>
+      <c r="B91" t="s">
+        <v>529</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D91">
+        <v>22</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1593</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>62</v>
+      </c>
+      <c r="B92" t="s">
+        <v>546</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D92">
+        <v>22</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" t="s">
+        <v>543</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D93">
+        <v>10</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1574</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>56</v>
+      </c>
+      <c r="B94" t="s">
+        <v>540</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D94">
+        <v>22</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>55</v>
+      </c>
+      <c r="B95" t="s">
+        <v>539</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D95">
+        <v>18</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" t="s">
+        <v>631</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D96">
+        <v>17</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>1442</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1582</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>1550</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>1617</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>626</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D97">
+        <v>12</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" t="s">
+        <v>629</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D98">
+        <v>32</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>181</v>
+      </c>
+      <c r="B99" t="s">
+        <v>813</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D99">
+        <v>13</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>1420</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>182</v>
+      </c>
+      <c r="B100" t="s">
+        <v>814</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D100">
+        <v>12</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>183</v>
+      </c>
+      <c r="B101" t="s">
+        <v>815</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D101">
+        <v>15</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" t="s">
+        <v>811</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D102">
+        <v>22</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" t="s">
+        <v>474</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D103">
+        <v>15</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104" t="s">
+        <v>521</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D104">
+        <v>26</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>1403</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1584</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>1552</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>1403</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>47</v>
+      </c>
+      <c r="B105" t="s">
+        <v>520</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D105">
+        <v>21</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1587</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>1553</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>176</v>
+      </c>
+      <c r="B106" t="s">
+        <v>804</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D106">
+        <v>23</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1593</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>175</v>
+      </c>
+      <c r="B107" t="s">
+        <v>802</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D107">
+        <v>13</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>1434</v>
+      </c>
+      <c r="F107" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>104</v>
+      </c>
+      <c r="B108" t="s">
+        <v>636</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D108">
+        <v>43</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>103</v>
+      </c>
+      <c r="B109" t="s">
+        <v>633</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D109">
+        <v>10</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F109" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>163</v>
+      </c>
+      <c r="B110" t="s">
+        <v>764</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D110">
+        <v>12</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H110" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>185</v>
+      </c>
+      <c r="B111" t="s">
+        <v>822</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D111">
+        <v>25</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F111" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H111" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>186</v>
+      </c>
+      <c r="B112" t="s">
+        <v>823</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D112">
+        <v>18</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F112" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>1556</v>
+      </c>
+      <c r="H112" s="4" t="s">
+        <v>1394</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>190</v>
+      </c>
+      <c r="B113" t="s">
+        <v>834</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D113">
+        <v>10</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1586</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>1558</v>
+      </c>
+      <c r="H113" s="4" t="s">
+        <v>1405</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" t="s">
+        <v>427</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D114">
+        <v>41</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>189</v>
+      </c>
+      <c r="B115" t="s">
+        <v>833</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D115">
+        <v>12</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F115" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H115" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="3"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="3"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="3"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="3"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="3"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="3"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" s="3"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="3"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="3"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="3"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="3"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="3"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="3"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="3"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="3"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="3"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="3"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="3"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="3"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="3"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="3"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="3"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="3"/>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A145" s="3"/>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A146" s="3"/>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A147" s="3"/>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A148" s="3"/>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A149" s="3"/>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A150" s="3"/>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A151" s="3"/>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A152" s="3"/>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A153" s="3"/>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A154" s="3"/>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A155" s="3"/>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A156" s="3"/>
+      <c r="O156" s="3"/>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A157" s="3"/>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A158" s="3"/>
+      <c r="N158" s="3"/>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A159" s="3"/>
+      <c r="N159" s="3"/>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A160" s="3"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="3"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3"/>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A161" s="3"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="3"/>
+      <c r="K161" s="3"/>
+      <c r="L161" s="3"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
+      <c r="O161" s="3"/>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A162" s="3"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="3"/>
+      <c r="K162" s="3"/>
+      <c r="L162" s="3"/>
+      <c r="M162" s="3"/>
+      <c r="N162" s="3"/>
+      <c r="O162" s="3"/>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A163" s="3"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
+      <c r="O163" s="3"/>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A164" s="3"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="3"/>
+      <c r="K164" s="3"/>
+      <c r="L164" s="3"/>
+      <c r="M164" s="3"/>
+      <c r="N164" s="3"/>
+      <c r="O164" s="3"/>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A165" s="3"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="3"/>
+      <c r="K165" s="3"/>
+      <c r="L165" s="3"/>
+      <c r="M165" s="3"/>
+      <c r="N165" s="3"/>
+      <c r="O165" s="3"/>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A166" s="3"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+      <c r="L166" s="3"/>
+      <c r="M166" s="3"/>
+      <c r="N166" s="3"/>
+      <c r="O166" s="3"/>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A167" s="3"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="3"/>
+      <c r="K167" s="3"/>
+      <c r="L167" s="3"/>
+      <c r="M167" s="3"/>
+      <c r="N167" s="3"/>
+      <c r="O167" s="3"/>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A168" s="3"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="3"/>
+      <c r="K168" s="3"/>
+      <c r="L168" s="3"/>
+      <c r="M168" s="3"/>
+      <c r="N168" s="3"/>
+      <c r="O168" s="3"/>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A169" s="3"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="3"/>
+      <c r="K169" s="3"/>
+      <c r="L169" s="3"/>
+      <c r="M169" s="3"/>
+      <c r="N169" s="3"/>
+      <c r="O169" s="3"/>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A170" s="3"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="3"/>
+      <c r="K170" s="3"/>
+      <c r="L170" s="3"/>
+      <c r="M170" s="3"/>
+      <c r="N170" s="3"/>
+      <c r="O170" s="3"/>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A171" s="3"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="3"/>
+      <c r="K171" s="3"/>
+      <c r="L171" s="3"/>
+      <c r="M171" s="3"/>
+      <c r="N171" s="3"/>
+      <c r="O171" s="3"/>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A172" s="3"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="3"/>
+      <c r="K172" s="3"/>
+      <c r="L172" s="3"/>
+      <c r="M172" s="3"/>
+      <c r="N172" s="3"/>
+      <c r="O172" s="3"/>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A173" s="3"/>
+      <c r="I173" s="3"/>
+      <c r="J173" s="3"/>
+      <c r="K173" s="3"/>
+      <c r="L173" s="3"/>
+      <c r="M173" s="3"/>
+      <c r="N173" s="3"/>
+      <c r="O173" s="3"/>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A174" s="3"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="3"/>
+      <c r="K174" s="3"/>
+      <c r="L174" s="3"/>
+      <c r="M174" s="3"/>
+      <c r="N174" s="3"/>
+      <c r="O174" s="3"/>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A175" s="3"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="3"/>
+      <c r="K175" s="3"/>
+      <c r="L175" s="3"/>
+      <c r="M175" s="3"/>
+      <c r="N175" s="3"/>
+      <c r="O175" s="3"/>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A176" s="3"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="3"/>
+      <c r="K176" s="3"/>
+      <c r="L176" s="3"/>
+      <c r="M176" s="3"/>
+      <c r="N176" s="3"/>
+      <c r="O176" s="3"/>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A177" s="3"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="3"/>
+      <c r="K177" s="3"/>
+      <c r="L177" s="3"/>
+      <c r="M177" s="3"/>
+      <c r="N177" s="3"/>
+      <c r="O177" s="3"/>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A178" s="3"/>
+      <c r="I178" s="3"/>
+      <c r="J178" s="3"/>
+      <c r="K178" s="3"/>
+      <c r="L178" s="3"/>
+      <c r="M178" s="3"/>
+      <c r="N178" s="3"/>
+      <c r="O178" s="3"/>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A179" s="3"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="3"/>
+      <c r="K179" s="3"/>
+      <c r="L179" s="3"/>
+      <c r="M179" s="3"/>
+      <c r="N179" s="3"/>
+      <c r="O179" s="3"/>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A180" s="3"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="3"/>
+      <c r="K180" s="3"/>
+      <c r="L180" s="3"/>
+      <c r="M180" s="3"/>
+      <c r="N180" s="3"/>
+      <c r="O180" s="3"/>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A181" s="3"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="3"/>
+      <c r="K181" s="3"/>
+      <c r="L181" s="3"/>
+      <c r="M181" s="3"/>
+      <c r="N181" s="3"/>
+      <c r="O181" s="3"/>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A182" s="3"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="3"/>
+      <c r="K182" s="3"/>
+      <c r="L182" s="3"/>
+      <c r="M182" s="3"/>
+      <c r="N182" s="3"/>
+      <c r="O182" s="3"/>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A183" s="3"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="3"/>
+      <c r="K183" s="3"/>
+      <c r="L183" s="3"/>
+      <c r="M183" s="3"/>
+      <c r="N183" s="3"/>
+      <c r="O183" s="3"/>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A184" s="3"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="3"/>
+      <c r="K184" s="3"/>
+      <c r="L184" s="3"/>
+      <c r="M184" s="3"/>
+      <c r="N184" s="3"/>
+      <c r="O184" s="3"/>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A185" s="3"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="3"/>
+      <c r="K185" s="3"/>
+      <c r="L185" s="3"/>
+      <c r="M185" s="3"/>
+      <c r="N185" s="3"/>
+      <c r="O185" s="3"/>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="3"/>
+      <c r="M186" s="3"/>
+      <c r="N186" s="3"/>
+      <c r="O186" s="3"/>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A187" s="3"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="3"/>
+      <c r="K187" s="3"/>
+      <c r="L187" s="3"/>
+      <c r="M187" s="3"/>
+      <c r="N187" s="3"/>
+      <c r="O187" s="3"/>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A188" s="3"/>
+      <c r="N188" s="3"/>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A189" s="3"/>
+      <c r="N189" s="3"/>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A190" s="3"/>
+      <c r="N190" s="3"/>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A191" s="3"/>
+      <c r="N191" s="3"/>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A192" s="3"/>
+      <c r="N192" s="3"/>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A193" s="3"/>
+      <c r="N193" s="3"/>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A194" s="3"/>
+      <c r="N194" s="3"/>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A195" s="3"/>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A196" s="3"/>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A197" s="3"/>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A198" s="3"/>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A199" s="3"/>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A200" s="3"/>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A201" s="3"/>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A202" s="3"/>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A203" s="3"/>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A204" s="3"/>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A205" s="3"/>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A206" s="3"/>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A207" s="3"/>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A208" s="3"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="3"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="3"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="3"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="3"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="3"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="3"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="3"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="3"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="3"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="3"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="3"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="3"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="3"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="3"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="3"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="3"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" s="3"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" s="3"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="3"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" s="3"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" s="3"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" s="3"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" s="3"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" s="3"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" s="3"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" s="3"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" s="3"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" s="3"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" s="3"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" s="3"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" s="3"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" s="3"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" s="3"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" s="3"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" s="3"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" s="3"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" s="3"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" s="3"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" s="3"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" s="3"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" s="3"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="3"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" s="3"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" s="3"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" s="3"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" s="3"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" s="3"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" s="3"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" s="3"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" s="3"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" s="3"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" s="3"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" s="3"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" s="3"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" s="3"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" s="3"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" s="3"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" s="3"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" s="3"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" s="3"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" s="3"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" s="3"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" s="3"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" s="3"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" s="3"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" s="3"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" s="3"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" s="3"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" s="3"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" s="3"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" s="3"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" s="3"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" s="3"/>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" s="3"/>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" s="3"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" s="3"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" s="3"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" s="3"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" s="3"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" s="3"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="3"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="3"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="3"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="3"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="3"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="3"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="3"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="3"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="3"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="3"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="3"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="3"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="3"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="3"/>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="3"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="3"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="3"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="3"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="3"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="3"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="3"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="3"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="3"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" s="3"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" s="3"/>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" s="3"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" s="3"/>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" s="3"/>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" s="3"/>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" s="3"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" s="3"/>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" s="3"/>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" s="3"/>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" s="3"/>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" s="3"/>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" s="3"/>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" s="3"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326" s="3"/>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327" s="3"/>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328" s="3"/>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329" s="3"/>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330" s="3"/>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331" s="3"/>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332" s="3"/>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333" s="3"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334" s="3"/>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335" s="3"/>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336" s="3"/>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="3"/>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338" s="3"/>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339" s="3"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340" s="3"/>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341" s="3"/>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34753C89-CDE4-994A-BA22-A0E4DAD6E05E}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A2:A10"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update to excel files
</commit_message>
<xml_diff>
--- a/docs/amps_prediction.xlsx
+++ b/docs/amps_prediction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome_2025/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A36E8EC-E99B-EE41-92AD-197570EEFC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4F4603-4A2F-854D-8002-8BBD54A0A938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{D0FE8B26-41E0-2A46-B2EA-AAB3A158C054}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{D0FE8B26-41E0-2A46-B2EA-AAB3A158C054}"/>
   </bookViews>
   <sheets>
     <sheet name="420_AMPs" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4992" uniqueCount="1625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4976" uniqueCount="1625">
   <si>
     <t>transcript_id</t>
   </si>
@@ -4922,7 +4922,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4978,6 +4978,19 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4999,7 +5012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5008,6 +5021,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9995,7 +10010,7 @@
   <dimension ref="A1:N420"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G194"/>
+      <selection activeCell="K5" sqref="J1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10006,6 +10021,7 @@
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -10031,7 +10047,8 @@
         <v>1460</v>
       </c>
       <c r="I1" s="2"/>
-      <c r="K1" s="5"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -10059,7 +10076,8 @@
         <v>1538</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="K2" s="5"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -10084,7 +10102,8 @@
         <v>1505</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="K3" s="5"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -10109,7 +10128,8 @@
         <v>1477</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="K4" s="5"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -10134,7 +10154,8 @@
         <v>1477</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="K5" s="5"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -15550,10 +15571,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C185CF0-F8B0-3943-BB47-B713145B4CF9}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G1:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15561,9 +15582,11 @@
     <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15582,8 +15605,10 @@
       <c r="F1" s="1" t="s">
         <v>1421</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -15602,8 +15627,10 @@
       <c r="F2" t="s">
         <v>1401</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -15622,8 +15649,10 @@
       <c r="F3" t="s">
         <v>1386</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>185</v>
       </c>
@@ -15642,8 +15671,10 @@
       <c r="F4" t="s">
         <v>1386</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>71</v>
       </c>
@@ -15662,8 +15693,10 @@
       <c r="F5" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>57</v>
       </c>
@@ -15683,7 +15716,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>94</v>
       </c>
@@ -15702,8 +15735,10 @@
       <c r="F7" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -15722,8 +15757,9 @@
       <c r="F8" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>145</v>
       </c>
@@ -15742,8 +15778,9 @@
       <c r="F9" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>159</v>
       </c>
@@ -15762,8 +15799,9 @@
       <c r="F10" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>131</v>
       </c>
@@ -15782,8 +15820,9 @@
       <c r="F11" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>104</v>
       </c>
@@ -15803,7 +15842,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>111</v>
       </c>
@@ -15823,7 +15862,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>74</v>
       </c>
@@ -15843,7 +15882,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>83</v>
       </c>
@@ -15863,7 +15902,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>94</v>
       </c>
@@ -22519,10 +22558,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A837C33-E513-FD45-9224-A40C02E07EC8}">
-  <dimension ref="A1:O342"/>
+  <dimension ref="A1:S340"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22533,9 +22572,10 @@
     <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -22563,11 +22603,15 @@
       <c r="I1" s="1" t="s">
         <v>1619</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -22595,8 +22639,15 @@
       <c r="I2" s="1" t="s">
         <v>1432</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>195</v>
       </c>
@@ -22624,8 +22675,15 @@
       <c r="I3" s="1" t="s">
         <v>1395</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -22653,9 +22711,15 @@
       <c r="I4" s="1" t="s">
         <v>1617</v>
       </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -22683,9 +22747,8 @@
       <c r="I5" s="1" t="s">
         <v>1620</v>
       </c>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -22714,7 +22777,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -22743,7 +22806,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -22772,7 +22835,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -22802,7 +22865,7 @@
       </c>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -22831,7 +22894,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -22860,7 +22923,7 @@
         <v>1621</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -22889,7 +22952,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -22918,7 +22981,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -22947,140 +23010,140 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1329</v>
-      </c>
-      <c r="D15" s="1">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>461</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D15">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>594</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D16">
         <v>10</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>1393</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>1581</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>1487</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>461</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1240</v>
-      </c>
-      <c r="D16">
-        <v>35</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>1410</v>
+        <v>1391</v>
       </c>
       <c r="F16" t="s">
-        <v>1594</v>
+        <v>1567</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>1483</v>
+        <v>1490</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>1410</v>
+        <v>1391</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1410</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>594</v>
+        <v>696</v>
       </c>
       <c r="C17" t="s">
-        <v>1293</v>
+        <v>1333</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>1391</v>
+        <v>1436</v>
       </c>
       <c r="F17" t="s">
-        <v>1567</v>
+        <v>1573</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>1567</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C18" t="s">
-        <v>1333</v>
+        <v>882</v>
       </c>
       <c r="D18">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>1436</v>
+        <v>1410</v>
       </c>
       <c r="F18" t="s">
-        <v>1573</v>
+        <v>1589</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>1392</v>
+        <v>1410</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1392</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>697</v>
+        <v>550</v>
       </c>
       <c r="C19" t="s">
-        <v>882</v>
+        <v>1277</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="F19" t="s">
-        <v>1589</v>
+        <v>1596</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>1483</v>
@@ -23094,22 +23157,22 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C20" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D20">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="F20" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>1483</v>
@@ -23123,402 +23186,402 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>551</v>
+        <v>781</v>
       </c>
       <c r="C21" t="s">
-        <v>1278</v>
+        <v>887</v>
       </c>
       <c r="D21">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>1410</v>
+        <v>1456</v>
       </c>
       <c r="F21" t="s">
-        <v>1594</v>
+        <v>1599</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>1483</v>
+        <v>1495</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>1410</v>
+        <v>1414</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>1410</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
-        <v>781</v>
+        <v>762</v>
       </c>
       <c r="C22" t="s">
-        <v>887</v>
+        <v>1359</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>1456</v>
+        <v>1393</v>
       </c>
       <c r="F22" t="s">
-        <v>1599</v>
+        <v>1563</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>1414</v>
+        <v>1393</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>1414</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>762</v>
+        <v>695</v>
       </c>
       <c r="C23" t="s">
-        <v>1359</v>
+        <v>1332</v>
       </c>
       <c r="D23">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>1393</v>
+        <v>1433</v>
       </c>
       <c r="F23" t="s">
-        <v>1563</v>
+        <v>1570</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>1497</v>
+        <v>1499</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
-        <v>695</v>
+        <v>753</v>
       </c>
       <c r="C24" t="s">
-        <v>1332</v>
+        <v>1357</v>
       </c>
       <c r="D24">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1433</v>
+        <v>1454</v>
       </c>
       <c r="F24" t="s">
-        <v>1570</v>
+        <v>1566</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>1499</v>
+        <v>1501</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>1389</v>
+        <v>1614</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>1389</v>
+        <v>1614</v>
       </c>
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
-        <v>753</v>
+        <v>737</v>
       </c>
       <c r="C25" t="s">
-        <v>1357</v>
+        <v>1349</v>
       </c>
       <c r="D25">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>1454</v>
+        <v>1393</v>
       </c>
       <c r="F25" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>1614</v>
+        <v>1386</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>1614</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>737</v>
+        <v>595</v>
       </c>
       <c r="C26" t="s">
-        <v>1349</v>
+        <v>1294</v>
       </c>
       <c r="D26">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>1393</v>
+        <v>1439</v>
       </c>
       <c r="F26" t="s">
-        <v>1563</v>
+        <v>1581</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>1386</v>
+        <v>1409</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1563</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>595</v>
+        <v>614</v>
       </c>
       <c r="C27" t="s">
-        <v>1294</v>
+        <v>1302</v>
       </c>
       <c r="D27">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>1439</v>
+        <v>1413</v>
       </c>
       <c r="F27" t="s">
-        <v>1581</v>
+        <v>1598</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>1503</v>
+        <v>1505</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>1409</v>
+        <v>1413</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>1439</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C28" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D28">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>1413</v>
+        <v>1419</v>
       </c>
       <c r="F28" t="s">
-        <v>1598</v>
+        <v>1608</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>1505</v>
+        <v>1507</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>1413</v>
+        <v>1417</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>1413</v>
+        <v>1417</v>
       </c>
       <c r="O28" s="3"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>615</v>
+        <v>809</v>
       </c>
       <c r="C29" t="s">
-        <v>1303</v>
+        <v>901</v>
       </c>
       <c r="D29">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>1419</v>
+        <v>1410</v>
       </c>
       <c r="F29" t="s">
-        <v>1608</v>
+        <v>1594</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>1507</v>
+        <v>1483</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>1417</v>
+        <v>1410</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>1417</v>
+        <v>1410</v>
       </c>
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
-        <v>809</v>
+        <v>763</v>
       </c>
       <c r="C30" t="s">
-        <v>901</v>
+        <v>1360</v>
       </c>
       <c r="D30">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>1410</v>
+        <v>1455</v>
       </c>
       <c r="F30" t="s">
-        <v>1594</v>
+        <v>1564</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>1483</v>
+        <v>1502</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>1410</v>
+        <v>1386</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1410</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>763</v>
+        <v>526</v>
       </c>
       <c r="C31" t="s">
-        <v>1360</v>
+        <v>1265</v>
       </c>
       <c r="D31">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>1455</v>
+        <v>1435</v>
       </c>
       <c r="F31" t="s">
-        <v>1564</v>
+        <v>1600</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>1502</v>
+        <v>1510</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>1386</v>
+        <v>1415</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>1564</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>526</v>
+        <v>493</v>
       </c>
       <c r="C32" t="s">
-        <v>1265</v>
+        <v>1250</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>1435</v>
+        <v>1429</v>
       </c>
       <c r="F32" t="s">
-        <v>1600</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>1510</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>1415</v>
+        <v>1607</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>1612</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>1415</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>493</v>
+        <v>765</v>
       </c>
       <c r="C33" t="s">
-        <v>1250</v>
+        <v>1361</v>
       </c>
       <c r="D33">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>1429</v>
+        <v>1410</v>
       </c>
       <c r="F33" t="s">
-        <v>1607</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>1612</v>
+        <v>1590</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>1410</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>1607</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C34" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D34">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="F34" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>1483</v>
@@ -23532,16 +23595,16 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>766</v>
+        <v>612</v>
       </c>
       <c r="C35" t="s">
-        <v>1362</v>
+        <v>1301</v>
       </c>
       <c r="D35">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>1410</v>
@@ -23561,22 +23624,22 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C36" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D36">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F36" t="s">
-        <v>1589</v>
+        <v>1593</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>1483</v>
@@ -23590,99 +23653,99 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>611</v>
+        <v>642</v>
       </c>
       <c r="C37" t="s">
-        <v>1300</v>
+        <v>1311</v>
       </c>
       <c r="D37">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>1423</v>
+        <v>1443</v>
       </c>
       <c r="F37" t="s">
-        <v>1593</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>1410</v>
+        <v>1606</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>1612</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>1410</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="B38" t="s">
-        <v>642</v>
+        <v>742</v>
       </c>
       <c r="C38" t="s">
-        <v>1311</v>
+        <v>1352</v>
       </c>
       <c r="D38">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>1443</v>
+        <v>1404</v>
       </c>
       <c r="F38" t="s">
-        <v>1606</v>
+        <v>1602</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>1462</v>
+        <v>1464</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>1612</v>
+        <v>1615</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>742</v>
+        <v>655</v>
       </c>
       <c r="C39" t="s">
-        <v>1352</v>
+        <v>1315</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>1404</v>
+        <v>1446</v>
       </c>
       <c r="F39" t="s">
-        <v>1602</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>1464</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>1615</v>
+        <v>1588</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>1518</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>1408</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>1623</v>
+        <v>1446</v>
       </c>
       <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C40" t="s">
         <v>1315</v>
@@ -23709,52 +23772,52 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
-        <v>656</v>
+        <v>745</v>
       </c>
       <c r="C41" t="s">
-        <v>1315</v>
+        <v>1355</v>
       </c>
       <c r="D41">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>1446</v>
+        <v>1423</v>
       </c>
       <c r="F41" t="s">
-        <v>1588</v>
+        <v>1590</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>1518</v>
+        <v>1483</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>1446</v>
+        <v>1410</v>
       </c>
       <c r="O41" s="3"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B42" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
       <c r="C42" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D42">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="F42" t="s">
-        <v>1590</v>
+        <v>1594</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>1483</v>
@@ -23769,200 +23832,200 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B43" t="s">
-        <v>750</v>
+        <v>757</v>
       </c>
       <c r="C43" t="s">
-        <v>1356</v>
+        <v>1358</v>
       </c>
       <c r="D43">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>1410</v>
+        <v>1418</v>
       </c>
       <c r="F43" t="s">
-        <v>1594</v>
+        <v>1610</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>1483</v>
+        <v>1523</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>1410</v>
+        <v>1418</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>1410</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>757</v>
+        <v>599</v>
       </c>
       <c r="C44" t="s">
-        <v>1358</v>
+        <v>1296</v>
       </c>
       <c r="D44">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>1418</v>
+        <v>1410</v>
       </c>
       <c r="F44" t="s">
-        <v>1610</v>
+        <v>1589</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>1523</v>
+        <v>1483</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>1418</v>
+        <v>1410</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>1418</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>599</v>
+        <v>429</v>
       </c>
       <c r="C45" t="s">
-        <v>1296</v>
+        <v>1228</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>1410</v>
+        <v>1424</v>
       </c>
       <c r="F45" t="s">
-        <v>1589</v>
+        <v>1565</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>1483</v>
+        <v>1526</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>1410</v>
+        <v>1387</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>1410</v>
+        <v>1565</v>
       </c>
       <c r="O45" s="3"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C46" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D46">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>1424</v>
+        <v>1416</v>
       </c>
       <c r="F46" t="s">
-        <v>1565</v>
+        <v>1601</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>1526</v>
+        <v>1528</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>1387</v>
+        <v>1416</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>1565</v>
+        <v>1416</v>
       </c>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>430</v>
+        <v>459</v>
       </c>
       <c r="C47" t="s">
-        <v>1229</v>
+        <v>1239</v>
       </c>
       <c r="D47">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="F47" t="s">
-        <v>1601</v>
+        <v>1597</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>1528</v>
+        <v>1505</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="O47" s="3"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C48" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="D48">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="F48" t="s">
-        <v>1597</v>
+        <v>1589</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>1505</v>
+        <v>1483</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="O48" s="3"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>458</v>
+        <v>496</v>
       </c>
       <c r="C49" t="s">
-        <v>1238</v>
+        <v>1252</v>
       </c>
       <c r="D49">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F49" t="s">
-        <v>1589</v>
+        <v>1591</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>1483</v>
@@ -23976,81 +24039,81 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C50" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="D50">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>1423</v>
+        <v>1391</v>
       </c>
       <c r="F50" t="s">
-        <v>1591</v>
+        <v>1568</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>1483</v>
+        <v>1499</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>1410</v>
+        <v>1389</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>1410</v>
+        <v>1389</v>
       </c>
       <c r="O50" s="3"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>495</v>
+        <v>727</v>
       </c>
       <c r="C51" t="s">
-        <v>1251</v>
+        <v>1342</v>
       </c>
       <c r="D51">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>1391</v>
+        <v>1394</v>
       </c>
       <c r="F51" t="s">
-        <v>1568</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>1499</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>1389</v>
+        <v>1603</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>1612</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>1389</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B52" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="C52" t="s">
-        <v>1342</v>
+        <v>1346</v>
       </c>
       <c r="D52">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>1394</v>
+        <v>1431</v>
       </c>
       <c r="F52" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>1462</v>
@@ -24059,401 +24122,401 @@
         <v>1612</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>1432</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C53" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="D53">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>1431</v>
+        <v>1419</v>
       </c>
       <c r="F53" t="s">
-        <v>1604</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>1612</v>
+        <v>1609</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>1417</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>1408</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>729</v>
+        <v>434</v>
       </c>
       <c r="C54" t="s">
-        <v>1343</v>
+        <v>1231</v>
       </c>
       <c r="D54">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>1419</v>
+        <v>1410</v>
       </c>
       <c r="F54" t="s">
-        <v>1609</v>
+        <v>1589</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>1507</v>
+        <v>1483</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>1417</v>
+        <v>1410</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>1417</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C55" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D55">
         <v>13</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>1410</v>
+        <v>1426</v>
       </c>
       <c r="F55" t="s">
-        <v>1589</v>
+        <v>1573</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>1483</v>
+        <v>1486</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>1410</v>
+        <v>1392</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>1410</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="C56" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D56">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="F56" t="s">
-        <v>1573</v>
+        <v>1590</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>1392</v>
+        <v>1410</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>1392</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C57" t="s">
-        <v>1233</v>
+        <v>1005</v>
       </c>
       <c r="D57">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="F57" t="s">
-        <v>1590</v>
+        <v>1611</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>1410</v>
+        <v>1419</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>1410</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>443</v>
+        <v>610</v>
       </c>
       <c r="C58" t="s">
-        <v>1005</v>
+        <v>1299</v>
       </c>
       <c r="D58">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>1419</v>
+        <v>1441</v>
       </c>
       <c r="F58" t="s">
-        <v>1611</v>
+        <v>1578</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>1479</v>
+        <v>1536</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>1419</v>
+        <v>1396</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>1419</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>610</v>
+        <v>739</v>
       </c>
       <c r="C59" t="s">
-        <v>1299</v>
+        <v>1351</v>
       </c>
       <c r="D59">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>1441</v>
+        <v>1410</v>
       </c>
       <c r="F59" t="s">
-        <v>1578</v>
+        <v>1592</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>1536</v>
+        <v>1483</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>1396</v>
+        <v>1410</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>1396</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>739</v>
+        <v>553</v>
       </c>
       <c r="C60" t="s">
-        <v>1351</v>
+        <v>1279</v>
       </c>
       <c r="D60">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>1410</v>
+        <v>1437</v>
       </c>
       <c r="F60" t="s">
-        <v>1592</v>
+        <v>1585</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>1483</v>
+        <v>1538</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>1410</v>
+        <v>1616</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="B61" t="s">
-        <v>553</v>
+        <v>726</v>
       </c>
       <c r="C61" t="s">
-        <v>1279</v>
+        <v>1341</v>
       </c>
       <c r="D61">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>1437</v>
+        <v>1429</v>
       </c>
       <c r="F61" t="s">
-        <v>1585</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>1538</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>1616</v>
+        <v>1607</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>1612</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>1404</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>726</v>
+        <v>651</v>
       </c>
       <c r="C62" t="s">
-        <v>1341</v>
+        <v>1314</v>
       </c>
       <c r="D62">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>1429</v>
+        <v>1445</v>
       </c>
       <c r="F62" t="s">
-        <v>1607</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>1612</v>
+        <v>1567</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>1499</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>1389</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1607</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>651</v>
+        <v>571</v>
       </c>
       <c r="C63" t="s">
-        <v>1314</v>
+        <v>1286</v>
       </c>
       <c r="D63">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>1445</v>
+        <v>1390</v>
       </c>
       <c r="F63" t="s">
-        <v>1567</v>
+        <v>1572</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>1499</v>
+        <v>1541</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C64" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D64">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>1390</v>
+        <v>1438</v>
       </c>
       <c r="F64" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>1541</v>
+        <v>1499</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>570</v>
+        <v>646</v>
       </c>
       <c r="C65" t="s">
-        <v>1285</v>
+        <v>1313</v>
       </c>
       <c r="D65">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>1438</v>
+        <v>1410</v>
       </c>
       <c r="F65" t="s">
-        <v>1569</v>
+        <v>1589</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>1499</v>
+        <v>1483</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C66" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D66">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F66" t="s">
         <v>1589</v>
@@ -24470,22 +24533,22 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>645</v>
+        <v>708</v>
       </c>
       <c r="C67" t="s">
-        <v>1312</v>
+        <v>1336</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="F67" t="s">
-        <v>1589</v>
+        <v>1595</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>1483</v>
@@ -24498,52 +24561,52 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="D68" s="1">
-        <v>21</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>1444</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>1561</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>1477</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>1613</v>
-      </c>
-      <c r="I68" s="7" t="s">
-        <v>1612</v>
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s">
+        <v>710</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D68">
+        <v>14</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>1452</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>1621</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>708</v>
+        <v>511</v>
       </c>
       <c r="C69" t="s">
-        <v>1336</v>
+        <v>1259</v>
       </c>
       <c r="D69">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F69" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>1483</v>
@@ -24557,51 +24620,51 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>710</v>
+        <v>510</v>
       </c>
       <c r="C70" t="s">
-        <v>1337</v>
+        <v>1258</v>
       </c>
       <c r="D70">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>1452</v>
+        <v>1427</v>
       </c>
       <c r="F70" t="s">
-        <v>1581</v>
+        <v>1603</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>1479</v>
+        <v>1539</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>1621</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="C71" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D71">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="F71" t="s">
-        <v>1591</v>
+        <v>1594</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>1483</v>
@@ -24615,51 +24678,51 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="C72" t="s">
-        <v>1258</v>
+        <v>1261</v>
       </c>
       <c r="D72">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>1427</v>
+        <v>1433</v>
       </c>
       <c r="F72" t="s">
-        <v>1603</v>
+        <v>1570</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>1539</v>
+        <v>1499</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>1420</v>
+        <v>1389</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>1427</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C73" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="D73">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="F73" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>1483</v>
@@ -24673,51 +24736,51 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="C74" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
       <c r="D74">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>1433</v>
+        <v>1410</v>
       </c>
       <c r="F74" t="s">
-        <v>1570</v>
+        <v>1591</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>1499</v>
+        <v>1483</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>508</v>
+        <v>668</v>
       </c>
       <c r="C75" t="s">
-        <v>1257</v>
+        <v>1320</v>
       </c>
       <c r="D75">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F75" t="s">
-        <v>1589</v>
+        <v>1592</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>1483</v>
@@ -24731,22 +24794,22 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="B76" t="s">
-        <v>505</v>
+        <v>671</v>
       </c>
       <c r="C76" t="s">
-        <v>1255</v>
+        <v>1322</v>
       </c>
       <c r="D76">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="F76" t="s">
-        <v>1591</v>
+        <v>1594</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>1483</v>
@@ -24760,51 +24823,51 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C77" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D77">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="F77" t="s">
-        <v>1592</v>
+        <v>1604</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>1410</v>
+        <v>1419</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>1410</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B78" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="C78" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="F78" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>1483</v>
@@ -24818,51 +24881,51 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B79" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="C79" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="D79">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>1419</v>
+        <v>1423</v>
       </c>
       <c r="F79" t="s">
-        <v>1604</v>
+        <v>1589</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>1479</v>
+        <v>1483</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>1419</v>
+        <v>1410</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1419</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="C80" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D80">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F80" t="s">
-        <v>1589</v>
+        <v>1592</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>1483</v>
@@ -24876,19 +24939,19 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B81" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C81" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="D81">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="F81" t="s">
         <v>1589</v>
@@ -24905,51 +24968,51 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="B82" t="s">
-        <v>676</v>
+        <v>792</v>
       </c>
       <c r="C82" t="s">
-        <v>1324</v>
+        <v>1364</v>
       </c>
       <c r="D82">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>1423</v>
+        <v>1412</v>
       </c>
       <c r="F82" t="s">
-        <v>1592</v>
+        <v>1581</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>1483</v>
+        <v>1546</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>1410</v>
+        <v>1412</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>1410</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="B83" t="s">
-        <v>677</v>
+        <v>789</v>
       </c>
       <c r="C83" t="s">
-        <v>1325</v>
+        <v>1363</v>
       </c>
       <c r="D83">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F83" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>1483</v>
@@ -24963,51 +25026,51 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>792</v>
+        <v>488</v>
       </c>
       <c r="C84" t="s">
-        <v>1364</v>
+        <v>1248</v>
       </c>
       <c r="D84">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="F84" t="s">
-        <v>1581</v>
+        <v>1589</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>1546</v>
+        <v>1483</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="B85" t="s">
-        <v>789</v>
+        <v>585</v>
       </c>
       <c r="C85" t="s">
-        <v>1363</v>
+        <v>1291</v>
       </c>
       <c r="D85">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>1423</v>
       </c>
       <c r="F85" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>1483</v>
@@ -25021,277 +25084,277 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B86" t="s">
-        <v>488</v>
+        <v>541</v>
       </c>
       <c r="C86" t="s">
-        <v>1248</v>
+        <v>1271</v>
       </c>
       <c r="D86">
         <v>29</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>1410</v>
+        <v>1427</v>
       </c>
       <c r="F86" t="s">
-        <v>1589</v>
+        <v>1603</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>1483</v>
+        <v>1539</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>1410</v>
+        <v>1420</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>1410</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B87" t="s">
-        <v>585</v>
+        <v>542</v>
       </c>
       <c r="C87" t="s">
-        <v>1291</v>
+        <v>1271</v>
       </c>
       <c r="D87">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>1423</v>
+        <v>1427</v>
       </c>
       <c r="F87" t="s">
-        <v>1591</v>
+        <v>1603</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>1483</v>
+        <v>1539</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>1410</v>
+        <v>1420</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1410</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B88" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="C88" t="s">
-        <v>1271</v>
+        <v>1266</v>
       </c>
       <c r="D88">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>1427</v>
+        <v>1391</v>
       </c>
       <c r="F88" t="s">
-        <v>1603</v>
+        <v>1567</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>1539</v>
+        <v>1499</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>1420</v>
+        <v>1389</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>1427</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B89" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="C89" t="s">
-        <v>1271</v>
+        <v>1133</v>
       </c>
       <c r="D89">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>1427</v>
+        <v>1410</v>
       </c>
       <c r="F89" t="s">
-        <v>1603</v>
+        <v>1593</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>1539</v>
+        <v>1483</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>1420</v>
+        <v>1410</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>1427</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B90" t="s">
-        <v>528</v>
+        <v>546</v>
       </c>
       <c r="C90" t="s">
-        <v>1266</v>
+        <v>1275</v>
       </c>
       <c r="D90">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>1391</v>
+        <v>1423</v>
       </c>
       <c r="F90" t="s">
-        <v>1567</v>
+        <v>1591</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>1499</v>
+        <v>1483</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B91" t="s">
-        <v>529</v>
+        <v>543</v>
       </c>
       <c r="C91" t="s">
-        <v>1133</v>
+        <v>1272</v>
       </c>
       <c r="D91">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>1410</v>
+        <v>1436</v>
       </c>
       <c r="F91" t="s">
-        <v>1593</v>
+        <v>1574</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>1483</v>
+        <v>1486</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>1410</v>
+        <v>1392</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>1410</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="C92" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="D92">
         <v>22</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>1423</v>
+        <v>1427</v>
       </c>
       <c r="F92" t="s">
-        <v>1591</v>
+        <v>1581</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>1410</v>
+        <v>1419</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>1410</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B93" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C93" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="D93">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>1436</v>
+        <v>1423</v>
       </c>
       <c r="F93" t="s">
-        <v>1574</v>
+        <v>1590</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>1392</v>
+        <v>1410</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>1392</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B94" t="s">
-        <v>540</v>
+        <v>631</v>
       </c>
       <c r="C94" t="s">
-        <v>1270</v>
+        <v>1309</v>
       </c>
       <c r="D94">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>1427</v>
+        <v>1442</v>
       </c>
       <c r="F94" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>1479</v>
+        <v>1550</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>1419</v>
+        <v>1617</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>1624</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>539</v>
+        <v>626</v>
       </c>
       <c r="C95" t="s">
-        <v>1269</v>
+        <v>1305</v>
       </c>
       <c r="D95">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>1423</v>
@@ -25311,80 +25374,80 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C96" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="D96">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>1442</v>
+        <v>1410</v>
       </c>
       <c r="F96" t="s">
-        <v>1582</v>
+        <v>1594</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>1550</v>
+        <v>1483</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>1617</v>
+        <v>1410</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>1617</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>181</v>
       </c>
       <c r="B97" t="s">
-        <v>626</v>
+        <v>813</v>
       </c>
       <c r="C97" t="s">
-        <v>1305</v>
+        <v>1373</v>
       </c>
       <c r="D97">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>1423</v>
+        <v>1427</v>
       </c>
       <c r="F97" t="s">
-        <v>1590</v>
+        <v>1603</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>1483</v>
+        <v>1539</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>1410</v>
+        <v>1420</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>1410</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="B98" t="s">
-        <v>629</v>
+        <v>814</v>
       </c>
       <c r="C98" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="D98">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="F98" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>1483</v>
@@ -25398,51 +25461,51 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B99" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C99" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D99">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="F99" t="s">
-        <v>1603</v>
+        <v>1591</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>1539</v>
+        <v>1483</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>1420</v>
+        <v>1410</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>1427</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C100" t="s">
-        <v>1305</v>
+        <v>1371</v>
       </c>
       <c r="D100">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="F100" t="s">
-        <v>1590</v>
+        <v>1592</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>1483</v>
@@ -25456,13 +25519,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>183</v>
+        <v>26</v>
       </c>
       <c r="B101" t="s">
-        <v>815</v>
+        <v>474</v>
       </c>
       <c r="C101" t="s">
-        <v>1374</v>
+        <v>1245</v>
       </c>
       <c r="D101">
         <v>15</v>
@@ -25485,167 +25548,167 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>811</v>
+        <v>521</v>
       </c>
       <c r="C102" t="s">
-        <v>1371</v>
+        <v>1264</v>
       </c>
       <c r="D102">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>1410</v>
+        <v>1403</v>
       </c>
       <c r="F102" t="s">
-        <v>1592</v>
+        <v>1584</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>1483</v>
+        <v>1552</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>1410</v>
+        <v>1403</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>1410</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B103" t="s">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c r="C103" t="s">
-        <v>1245</v>
+        <v>1263</v>
       </c>
       <c r="D103">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>1423</v>
+        <v>1406</v>
       </c>
       <c r="F103" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>1483</v>
+        <v>1553</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>1410</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>521</v>
+        <v>804</v>
       </c>
       <c r="C104" t="s">
-        <v>1264</v>
+        <v>1369</v>
       </c>
       <c r="D104">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>1403</v>
+        <v>1423</v>
       </c>
       <c r="F104" t="s">
-        <v>1584</v>
+        <v>1593</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>1552</v>
+        <v>1483</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>1403</v>
+        <v>1410</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>1403</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>47</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
-        <v>520</v>
+        <v>802</v>
       </c>
       <c r="C105" t="s">
-        <v>1263</v>
+        <v>1368</v>
       </c>
       <c r="D105">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>1406</v>
+        <v>1434</v>
       </c>
       <c r="F105" t="s">
-        <v>1587</v>
+        <v>1591</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>1553</v>
+        <v>1483</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>1406</v>
+        <v>1410</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>1617</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>176</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>804</v>
+        <v>636</v>
       </c>
       <c r="C106" t="s">
-        <v>1369</v>
+        <v>1310</v>
       </c>
       <c r="D106">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>1423</v>
+        <v>1433</v>
       </c>
       <c r="F106" t="s">
-        <v>1593</v>
+        <v>1571</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>1483</v>
+        <v>1499</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>1410</v>
+        <v>1389</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>1410</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>103</v>
       </c>
       <c r="B107" t="s">
-        <v>802</v>
+        <v>633</v>
       </c>
       <c r="C107" t="s">
-        <v>1368</v>
+        <v>1296</v>
       </c>
       <c r="D107">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>1434</v>
+        <v>1410</v>
       </c>
       <c r="F107" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>1483</v>
@@ -25659,45 +25722,45 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="B108" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="C108" t="s">
-        <v>1310</v>
+        <v>1305</v>
       </c>
       <c r="D108">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>1433</v>
+        <v>1423</v>
       </c>
       <c r="F108" t="s">
-        <v>1571</v>
+        <v>1590</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>1499</v>
+        <v>1483</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>1389</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="B109" t="s">
-        <v>633</v>
+        <v>822</v>
       </c>
       <c r="C109" t="s">
-        <v>1296</v>
+        <v>1375</v>
       </c>
       <c r="D109">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>1410</v>
@@ -25717,177 +25780,125 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="B110" t="s">
-        <v>764</v>
+        <v>823</v>
       </c>
       <c r="C110" t="s">
-        <v>1305</v>
+        <v>1376</v>
       </c>
       <c r="D110">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="F110" t="s">
-        <v>1590</v>
+        <v>1575</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>1483</v>
+        <v>1556</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>1410</v>
+        <v>1394</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>1410</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
-        <v>822</v>
+        <v>834</v>
       </c>
       <c r="C111" t="s">
-        <v>1375</v>
+        <v>1379</v>
       </c>
       <c r="D111">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>1410</v>
+        <v>1449</v>
       </c>
       <c r="F111" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>1483</v>
+        <v>1558</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>1410</v>
+        <v>1405</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>1410</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>186</v>
+        <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>823</v>
+        <v>427</v>
       </c>
       <c r="C112" t="s">
-        <v>1376</v>
+        <v>1227</v>
       </c>
       <c r="D112">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>1410</v>
+        <v>1418</v>
       </c>
       <c r="F112" t="s">
-        <v>1575</v>
-      </c>
-      <c r="G112" s="4" t="s">
-        <v>1556</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>1394</v>
+        <v>1603</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>1612</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>1575</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C113" t="s">
-        <v>1379</v>
+        <v>1224</v>
       </c>
       <c r="D113">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>1449</v>
+        <v>1423</v>
       </c>
       <c r="F113" t="s">
-        <v>1586</v>
+        <v>1591</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>1558</v>
+        <v>1483</v>
       </c>
       <c r="H113" s="4" t="s">
-        <v>1405</v>
+        <v>1410</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>1405</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>4</v>
-      </c>
-      <c r="B114" t="s">
-        <v>427</v>
-      </c>
-      <c r="C114" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D114">
-        <v>41</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>1418</v>
-      </c>
-      <c r="F114" t="s">
-        <v>1603</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H114" s="6" t="s">
-        <v>1612</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>1432</v>
-      </c>
+      <c r="A114" s="3"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>189</v>
-      </c>
-      <c r="B115" t="s">
-        <v>833</v>
-      </c>
-      <c r="C115" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D115">
-        <v>12</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>1423</v>
-      </c>
-      <c r="F115" t="s">
-        <v>1591</v>
-      </c>
-      <c r="G115" s="4" t="s">
-        <v>1483</v>
-      </c>
-      <c r="H115" s="4" t="s">
-        <v>1410</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>1410</v>
-      </c>
+      <c r="A115" s="3"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
@@ -26018,10 +26029,12 @@
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
+      <c r="I158" s="3"/>
       <c r="N158" s="3"/>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
+      <c r="I159" s="3"/>
       <c r="N159" s="3"/>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.2">
@@ -26286,7 +26299,6 @@
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" s="3"/>
-      <c r="I186" s="3"/>
       <c r="J186" s="3"/>
       <c r="K186" s="3"/>
       <c r="L186" s="3"/>
@@ -26296,7 +26308,6 @@
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" s="3"/>
-      <c r="I187" s="3"/>
       <c r="J187" s="3"/>
       <c r="K187" s="3"/>
       <c r="L187" s="3"/>
@@ -26769,12 +26780,6 @@
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="3"/>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A341" s="3"/>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A342" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26786,8 +26791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34753C89-CDE4-994A-BA22-A0E4DAD6E05E}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>